<commit_message>
se actualiza inventario de pruebas exploratorias
</commit_message>
<xml_diff>
--- a/Ejecucion-Semana1/inventario-pruebas-exploratorias.xlsx
+++ b/Ejecucion-Semana1/inventario-pruebas-exploratorias.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIANDES\ciclo-ii-2022\pruebas-automatizadas\semana-1\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1298FE51-E916-41BA-998B-87BF64D2526A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC0CA160-53C3-4AEF-83EB-10C0790C5C30}" xr6:coauthVersionLast="48" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -103,6 +105,9 @@
     <t>PA001</t>
   </si>
   <si>
+    <t>Ingeniero Automatizador 1</t>
+  </si>
+  <si>
     <t>Login</t>
   </si>
   <si>
@@ -133,7 +138,7 @@
     <t>https://uniandes-my.sharepoint.com/:v:/g/personal/e_melara_uniandes_edu_co/EYDTpPLw-KBGjG-nMO4l690ByeNyfv0ikcz6WI3FixPeYw?e=bbcRLh</t>
   </si>
   <si>
-    <t>INC001</t>
+    <t>https://github.com/clts-uniandes/estrategia-pruebas-ghost/issues/13</t>
   </si>
   <si>
     <t>PA003</t>
@@ -160,7 +165,7 @@
     <t>https://uniandes-my.sharepoint.com/:v:/g/personal/e_melara_uniandes_edu_co/EQmiqDvuXwVCsel38L7U5dABvw-yhWgSEEBXzCVX51yFKw?e=H1hlJ2</t>
   </si>
   <si>
-    <t>INC002</t>
+    <t>https://github.com/clts-uniandes/estrategia-pruebas-ghost/issues/14</t>
   </si>
   <si>
     <t>PA005</t>
@@ -187,12 +192,15 @@
     <t>https://uniandes-my.sharepoint.com/:v:/g/personal/e_melara_uniandes_edu_co/EUtcYFZLPK5Etp626nXA2t0BhfcBpWd1ttReuWBv4Zcqkg?e=YtX2YJ</t>
   </si>
   <si>
-    <t>INC003</t>
+    <t>https://github.com/clts-uniandes/estrategia-pruebas-ghost/issues/15</t>
   </si>
   <si>
     <t>PA007</t>
   </si>
   <si>
+    <t>Ingeniero Automatizador 2</t>
+  </si>
+  <si>
     <t>Editar Tag</t>
   </si>
   <si>
@@ -211,7 +219,7 @@
     <t>https://uniandes-my.sharepoint.com/:v:/g/personal/e_melara_uniandes_edu_co/Eb_vljupJDVEu961a_0Che4BjxLdrcXIFtHkQQpWHpKxFA?e=CS4S68</t>
   </si>
   <si>
-    <t>INC004</t>
+    <t>https://github.com/clts-uniandes/estrategia-pruebas-ghost/issues/16</t>
   </si>
   <si>
     <t>PA009</t>
@@ -235,7 +243,7 @@
     <t>https://uniandes-my.sharepoint.com/:v:/g/personal/e_melara_uniandes_edu_co/ERQbuuMk8EJDjRhnNhGzXVABpoi0hpWuUVdZFBY_vCiIBw?e=c4s9Wl</t>
   </si>
   <si>
-    <t>INC005</t>
+    <t>https://github.com/clts-uniandes/estrategia-pruebas-ghost/issues/17</t>
   </si>
   <si>
     <t>PA011</t>
@@ -262,12 +270,15 @@
     <t>https://uniandes-my.sharepoint.com/:v:/g/personal/e_melara_uniandes_edu_co/EbWJigfuOxpKkA189U04uqQBMc2gwd2dYFKu7_OSRo_lng?e=TgPsNT</t>
   </si>
   <si>
-    <t>INC006</t>
+    <t>https://github.com/clts-uniandes/estrategia-pruebas-ghost/issues/18</t>
   </si>
   <si>
     <t>PA013</t>
   </si>
   <si>
+    <t>Ingeniero Automatizador 3</t>
+  </si>
+  <si>
     <t>Eliminar Tag</t>
   </si>
   <si>
@@ -286,7 +297,7 @@
     <t>https://uniandes-my.sharepoint.com/:v:/g/personal/e_melara_uniandes_edu_co/ES4bwzgfGl1NsJ-JOcuVyuEB6WBRFz7FtdGJxLwBKlxR5A?e=20y733</t>
   </si>
   <si>
-    <t>INC007</t>
+    <t>https://github.com/clts-uniandes/estrategia-pruebas-ghost/issues/19</t>
   </si>
   <si>
     <t>PA015</t>
@@ -307,7 +318,7 @@
     <t>https://uniandes-my.sharepoint.com/:v:/g/personal/e_melara_uniandes_edu_co/EY5Q8s-Wv2NNlEpHgKdqojkBiYuScaOq3GENCKKd7GOr-A?e=sXrYoq</t>
   </si>
   <si>
-    <t>INC008</t>
+    <t>https://github.com/clts-uniandes/estrategia-pruebas-ghost/issues/20</t>
   </si>
   <si>
     <t>PA017</t>
@@ -331,12 +342,15 @@
     <t>https://uniandes-my.sharepoint.com/:v:/g/personal/e_melara_uniandes_edu_co/ERQ2XgcrC5RHiIjZtI6AD3cBGbOXB_uSCzlHoR-Vx8M8oA?e=xqxUlO</t>
   </si>
   <si>
-    <t>INC009</t>
+    <t>https://github.com/clts-uniandes/estrategia-pruebas-ghost/issues/21</t>
   </si>
   <si>
     <t>PA019</t>
   </si>
   <si>
+    <t>Ingeniero Automatizador 4</t>
+  </si>
+  <si>
     <t>Crear Pagina</t>
   </si>
   <si>
@@ -358,7 +372,7 @@
     <t>https://uniandes-my.sharepoint.com/:v:/g/personal/e_melara_uniandes_edu_co/EbVu8icqD11LrAJzf8NkPNwBNTpQ7oxzEubnmJOsDq0F0w?e=gGM7pa</t>
   </si>
   <si>
-    <t>INC010</t>
+    <t>https://github.com/clts-uniandes/estrategia-pruebas-ghost/issues/10</t>
   </si>
   <si>
     <t>PA021</t>
@@ -382,7 +396,7 @@
     <t>https://uniandes-my.sharepoint.com/:v:/g/personal/e_melara_uniandes_edu_co/EQC09XcopItHiU_b7sdcX-QBGm6W1avAKOzHGa2gkIf_SQ?e=0lU9s3</t>
   </si>
   <si>
-    <t>INC011</t>
+    <t>https://github.com/clts-uniandes/estrategia-pruebas-ghost/issues/11</t>
   </si>
   <si>
     <t>PA023</t>
@@ -406,7 +420,7 @@
     <t>https://uniandes-my.sharepoint.com/:v:/g/personal/e_melara_uniandes_edu_co/EUcZiyPbjYJNr0FyMhxFI5ABCR97GWNMbLs5BTe1LPz0Og?e=mTnYs4</t>
   </si>
   <si>
-    <t>INC012</t>
+    <t>https://github.com/clts-uniandes/estrategia-pruebas-ghost/issues/12</t>
   </si>
   <si>
     <t>Nota: Para ver los videos se tiene que estar autenticado con Uniandes</t>
@@ -422,25 +436,13 @@
   </si>
   <si>
     <t>Mix</t>
-  </si>
-  <si>
-    <t>Ingeniero Automatizador 1</t>
-  </si>
-  <si>
-    <t>Ingeniero Automatizador 2</t>
-  </si>
-  <si>
-    <t>Ingeniero Automatizador 3</t>
-  </si>
-  <si>
-    <t>Ingeniero Automatizador 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -713,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -725,6 +727,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -752,25 +774,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -1109,11 +1112,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="68" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="I6" zoomScale="68" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="30.375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
@@ -1123,10 +1124,10 @@
     <col min="7" max="7" width="23.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="64" customWidth="1"/>
     <col min="9" max="9" width="129.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5" customWidth="1"/>
+    <col min="10" max="10" width="59.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1137,20 +1138,20 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="2:10">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+    </row>
+    <row r="3" spans="2:10">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1161,52 +1162,52 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="23.1" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="15"/>
-    </row>
-    <row r="5" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="2:10" ht="30.95" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-    </row>
-    <row r="6" spans="2:10" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="2:10" ht="114.75" customHeight="1">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="28"/>
+    </row>
+    <row r="7" spans="2:10">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1217,745 +1218,745 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="2:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+    </row>
+    <row r="9" spans="2:10" ht="47.25">
+      <c r="B9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+    <row r="10" spans="2:10">
+      <c r="B10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="19">
-        <v>44654</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="E10" s="20" t="s">
+      <c r="C10" s="10">
+        <v>44654</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="E10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="F10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="G10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="H10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="I10" s="12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
+      <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="C11" s="4">
         <v>44654</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>125</v>
+        <v>18</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="35.25" customHeight="1">
+      <c r="B13" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="17">
+        <v>44654</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="10">
+        <v>44654</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="H17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="26">
-        <v>44654</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="27" t="s">
+      <c r="F19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="17">
+        <v>44654</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="10">
+        <v>44654</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J25" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="17">
+        <v>44654</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="J15" s="29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="19">
-        <v>44654</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="I16" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="26">
-        <v>44654</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="J21" s="29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="19">
-        <v>44654</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="I22" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="J22" s="22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J24" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="J25" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="J26" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="26">
-        <v>44654</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G27" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="I27" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="J27" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="18" t="s">
+      <c r="F27" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="19">
-        <v>44654</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="E28" s="20" t="s">
+      <c r="I27" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="F28" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="20" t="s">
+      <c r="J27" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="I28" s="30" t="s">
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="J28" s="22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="23" t="s">
+      <c r="C28" s="10">
+        <v>44654</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>99</v>
       </c>
+      <c r="E28" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I28" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="14" t="s">
+        <v>103</v>
+      </c>
       <c r="C29" s="4">
         <v>44654</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="E29" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J29" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="4">
+        <v>44654</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="J29" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="C30" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="J30" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C31" s="4">
-        <v>44654</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="F31" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="J31" s="24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="23" t="s">
-        <v>112</v>
+        <v>114</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="14" t="s">
+        <v>116</v>
       </c>
       <c r="C32" s="4">
         <v>44654</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="J32" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="C33" s="26">
-        <v>44654</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="E33" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G33" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="H33" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="17">
+        <v>44654</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="I33" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="J33" s="29" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F33" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="I33" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="J33" s="22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1966,9 +1967,9 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10">
       <c r="B35" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1979,7 +1980,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1990,7 +1991,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2001,7 +2002,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2012,7 +2013,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2023,7 +2024,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2034,7 +2035,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2045,18 +2046,18 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
+    <row r="42" spans="2:10" ht="26.1" customHeight="1">
+      <c r="B42" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2093,10 +2094,22 @@
     <hyperlink ref="I28" r:id="rId22" xr:uid="{927229EB-683A-42D7-9BFB-7AAFDC09A999}"/>
     <hyperlink ref="I30" r:id="rId23" xr:uid="{C972E2DB-81A1-4843-86C8-26020B3FBE8F}"/>
     <hyperlink ref="I32" r:id="rId24" xr:uid="{5BA19FB1-C08E-4A26-959E-D68B3485CA39}"/>
+    <hyperlink ref="J11" r:id="rId25" xr:uid="{7AECF693-0B7D-457D-9611-E5A2A81E13A7}"/>
+    <hyperlink ref="J13" r:id="rId26" xr:uid="{74DAC7C7-5014-4411-986B-349826B460A6}"/>
+    <hyperlink ref="J15" r:id="rId27" xr:uid="{877E2828-6649-49AB-B44A-DB3EA3E69AA8}"/>
+    <hyperlink ref="J17" r:id="rId28" xr:uid="{D4C49DE1-FB1E-4126-A7B8-836B1E316575}"/>
+    <hyperlink ref="J19" r:id="rId29" xr:uid="{47D753C3-68FD-4A1A-8C3C-904E21CBE72C}"/>
+    <hyperlink ref="J21" r:id="rId30" xr:uid="{BF9B0920-81F7-469D-BC52-BAE9125C76CA}"/>
+    <hyperlink ref="J23" r:id="rId31" xr:uid="{F65CB120-2B8E-4446-A654-FFA39D9E0560}"/>
+    <hyperlink ref="J25" r:id="rId32" xr:uid="{1D5FA4A3-D87D-45D6-A64D-4879DDB08D8A}"/>
+    <hyperlink ref="J27" r:id="rId33" xr:uid="{CD21C90D-E11F-4625-953F-5BDD4DD21072}"/>
+    <hyperlink ref="J29" r:id="rId34" xr:uid="{49AD7885-072C-476F-B90D-EC5F567591B9}"/>
+    <hyperlink ref="J31" r:id="rId35" xr:uid="{96E8AA7F-CBD4-4637-8901-9902CBEB8485}"/>
+    <hyperlink ref="J33" r:id="rId36" xr:uid="{8490A30D-71BB-4C34-AF65-16E96CCBE897}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId25"/>
+  <drawing r:id="rId37"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -2126,41 +2139,41 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="11.625" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>